<commit_message>
Andrea's Project Merge & Luis' Additions
</commit_message>
<xml_diff>
--- a/Requisitos Bolsa de Trabajo.xlsx
+++ b/Requisitos Bolsa de Trabajo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\05. Integradora II\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05. Integradora II\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -277,8 +277,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,8 +308,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +359,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -365,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -403,12 +416,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +739,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,23 +776,23 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -824,7 +842,7 @@
       <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1058,7 +1076,7 @@
       <c r="J13" s="7">
         <v>61</v>
       </c>
-      <c r="K13" s="4"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="7" t="s">
         <v>29</v>
       </c>
@@ -1085,7 +1103,7 @@
       <c r="J14" s="7">
         <v>62</v>
       </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="23"/>
       <c r="L14" s="7" t="s">
         <v>31</v>
       </c>
@@ -1096,7 +1114,7 @@
       <c r="B15" s="7">
         <v>12</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="7" t="s">
         <v>32</v>
       </c>
@@ -1123,7 +1141,7 @@
       <c r="B16" s="7">
         <v>13</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="7" t="s">
         <v>35</v>
       </c>
@@ -1231,7 +1249,7 @@
       <c r="B20" s="7">
         <v>17</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="7" t="s">
         <v>47</v>
       </c>
@@ -1247,7 +1265,7 @@
       <c r="J20" s="7">
         <v>68</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="K20" s="5"/>
       <c r="L20" s="7" t="s">
         <v>49</v>
       </c>
@@ -1366,7 +1384,7 @@
       <c r="B25" s="7">
         <v>22</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="7" t="s">
         <v>59</v>
       </c>
@@ -1490,7 +1508,7 @@
       <c r="J29" s="7">
         <v>77</v>
       </c>
-      <c r="K29" s="4"/>
+      <c r="K29" s="5"/>
       <c r="L29" s="7" t="s">
         <v>69</v>
       </c>
@@ -1529,7 +1547,7 @@
         <v>76</v>
       </c>
       <c r="C31" s="15"/>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="19" t="s">
         <v>81</v>
       </c>
       <c r="E31" s="13"/>
@@ -1563,7 +1581,7 @@
       <c r="J32" s="13">
         <v>80</v>
       </c>
-      <c r="K32" s="15"/>
+      <c r="K32" s="22"/>
       <c r="L32" s="13" t="s">
         <v>72</v>
       </c>
@@ -1602,7 +1620,7 @@
         <v>76</v>
       </c>
       <c r="K34" s="15"/>
-      <c r="L34" s="20" t="s">
+      <c r="L34" s="19" t="s">
         <v>81</v>
       </c>
       <c r="M34" s="7"/>

</xml_diff>

<commit_message>
Daniela's Project Merge & Updated Excel
</commit_message>
<xml_diff>
--- a/Requisitos Bolsa de Trabajo.xlsx
+++ b/Requisitos Bolsa de Trabajo.xlsx
@@ -323,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +390,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -403,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -440,9 +446,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -459,6 +462,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,7 +778,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,23 +815,23 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -852,11 +859,11 @@
         <v>3</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>27</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="6"/>
@@ -882,7 +889,7 @@
       <c r="F5" s="6">
         <v>28</v>
       </c>
-      <c r="G5" s="23"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="6" t="s">
         <v>7</v>
       </c>
@@ -890,7 +897,7 @@
       <c r="J5" s="6">
         <v>53</v>
       </c>
-      <c r="K5" s="19"/>
+      <c r="K5" s="18"/>
       <c r="L5" s="6" t="s">
         <v>6</v>
       </c>
@@ -910,7 +917,7 @@
       <c r="F6" s="6">
         <v>29</v>
       </c>
-      <c r="G6" s="23"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
@@ -918,7 +925,7 @@
       <c r="J6" s="6">
         <v>54</v>
       </c>
-      <c r="K6" s="19"/>
+      <c r="K6" s="18"/>
       <c r="L6" s="6" t="s">
         <v>10</v>
       </c>
@@ -935,18 +942,18 @@
         <v>11</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>30</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24" t="s">
+      <c r="G7" s="23"/>
+      <c r="H7" s="23" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6">
         <v>55</v>
       </c>
-      <c r="K7" s="19"/>
+      <c r="K7" s="18"/>
       <c r="L7" s="6" t="s">
         <v>13</v>
       </c>
@@ -965,7 +972,7 @@
       <c r="F8" s="6">
         <v>31</v>
       </c>
-      <c r="G8" s="22"/>
+      <c r="G8" s="21"/>
       <c r="H8" s="6" t="s">
         <v>15</v>
       </c>
@@ -992,7 +999,7 @@
       <c r="F9" s="6">
         <v>32</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1000,7 +1007,7 @@
       <c r="J9" s="6">
         <v>57</v>
       </c>
-      <c r="K9" s="19"/>
+      <c r="K9" s="18"/>
       <c r="L9" s="6" t="s">
         <v>19</v>
       </c>
@@ -1011,7 +1018,7 @@
       <c r="B10" s="6">
         <v>7</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="6" t="s">
         <v>20</v>
       </c>
@@ -1019,7 +1026,7 @@
       <c r="F10" s="6">
         <v>33</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="21"/>
       <c r="H10" s="6" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1034,7 @@
       <c r="J10" s="6">
         <v>58</v>
       </c>
-      <c r="K10" s="19"/>
+      <c r="K10" s="18"/>
       <c r="L10" s="6" t="s">
         <v>16</v>
       </c>
@@ -1046,7 +1053,7 @@
       <c r="F11" s="6">
         <v>34</v>
       </c>
-      <c r="G11" s="22"/>
+      <c r="G11" s="21"/>
       <c r="H11" s="6" t="s">
         <v>23</v>
       </c>
@@ -1054,7 +1061,7 @@
       <c r="J11" s="6">
         <v>59</v>
       </c>
-      <c r="K11" s="19"/>
+      <c r="K11" s="18"/>
       <c r="L11" s="6" t="s">
         <v>24</v>
       </c>
@@ -1073,7 +1080,7 @@
       <c r="F12" s="6">
         <v>35</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="6" t="s">
         <v>26</v>
       </c>
@@ -1081,7 +1088,7 @@
       <c r="J12" s="6">
         <v>60</v>
       </c>
-      <c r="K12" s="19"/>
+      <c r="K12" s="18"/>
       <c r="L12" s="6" t="s">
         <v>27</v>
       </c>
@@ -1097,18 +1104,18 @@
         <v>24</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="24">
+      <c r="F13" s="23">
         <v>36</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24" t="s">
+      <c r="G13" s="23"/>
+      <c r="H13" s="23" t="s">
         <v>28</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6">
         <v>61</v>
       </c>
-      <c r="K13" s="19"/>
+      <c r="K13" s="18"/>
       <c r="L13" s="6" t="s">
         <v>29</v>
       </c>
@@ -1127,16 +1134,16 @@
       <c r="F14" s="6">
         <v>37</v>
       </c>
-      <c r="G14" s="25"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="6" t="s">
         <v>30</v>
       </c>
       <c r="I14" s="6"/>
-      <c r="J14" s="21">
+      <c r="J14" s="20">
         <v>62</v>
       </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21" t="s">
+      <c r="K14" s="20"/>
+      <c r="L14" s="20" t="s">
         <v>31</v>
       </c>
       <c r="M14" s="6"/>
@@ -1154,7 +1161,7 @@
       <c r="F15" s="6">
         <v>38</v>
       </c>
-      <c r="G15" s="25"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="6" t="s">
         <v>33</v>
       </c>
@@ -1181,7 +1188,7 @@
       <c r="F16" s="6">
         <v>39</v>
       </c>
-      <c r="G16" s="23"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="6" t="s">
         <v>36</v>
       </c>
@@ -1208,7 +1215,7 @@
       <c r="F17" s="6">
         <v>40</v>
       </c>
-      <c r="G17" s="23"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="6" t="s">
         <v>39</v>
       </c>
@@ -1232,11 +1239,11 @@
         <v>41</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="24">
+      <c r="F18" s="23">
         <v>41</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24" t="s">
+      <c r="G18" s="23"/>
+      <c r="H18" s="23" t="s">
         <v>42</v>
       </c>
       <c r="I18" s="6"/>
@@ -1262,7 +1269,7 @@
       <c r="F19" s="6">
         <v>42</v>
       </c>
-      <c r="G19" s="26"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="6" t="s">
         <v>45</v>
       </c>
@@ -1289,7 +1296,7 @@
       <c r="F20" s="6">
         <v>43</v>
       </c>
-      <c r="G20" s="26"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="6" t="s">
         <v>48</v>
       </c>
@@ -1297,7 +1304,7 @@
       <c r="J20" s="6">
         <v>68</v>
       </c>
-      <c r="K20" s="19"/>
+      <c r="K20" s="18"/>
       <c r="L20" s="6" t="s">
         <v>49</v>
       </c>
@@ -1316,7 +1323,7 @@
       <c r="F21" s="6">
         <v>44</v>
       </c>
-      <c r="G21" s="26"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="6" t="s">
         <v>51</v>
       </c>
@@ -1343,7 +1350,7 @@
       <c r="F22" s="6">
         <v>45</v>
       </c>
-      <c r="G22" s="26"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="6" t="s">
         <v>57</v>
       </c>
@@ -1351,7 +1358,7 @@
       <c r="J22" s="6">
         <v>70</v>
       </c>
-      <c r="K22" s="19"/>
+      <c r="K22" s="18"/>
       <c r="L22" s="6" t="s">
         <v>54</v>
       </c>
@@ -1370,7 +1377,7 @@
       <c r="F23" s="6">
         <v>46</v>
       </c>
-      <c r="G23" s="26"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="6" t="s">
         <v>60</v>
       </c>
@@ -1378,7 +1385,7 @@
       <c r="J23" s="6">
         <v>71</v>
       </c>
-      <c r="K23" s="19"/>
+      <c r="K23" s="18"/>
       <c r="L23" s="6" t="s">
         <v>46</v>
       </c>
@@ -1397,7 +1404,7 @@
       <c r="F24" s="6">
         <v>47</v>
       </c>
-      <c r="G24" s="26"/>
+      <c r="G24" s="25"/>
       <c r="H24" s="6" t="s">
         <v>63</v>
       </c>
@@ -1405,7 +1412,7 @@
       <c r="J24" s="6">
         <v>72</v>
       </c>
-      <c r="K24" s="19"/>
+      <c r="K24" s="18"/>
       <c r="L24" s="6" t="s">
         <v>58</v>
       </c>
@@ -1421,11 +1428,11 @@
         <v>59</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="24">
+      <c r="F25" s="23">
         <v>48</v>
       </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24" t="s">
+      <c r="G25" s="23"/>
+      <c r="H25" s="23" t="s">
         <v>64</v>
       </c>
       <c r="I25" s="6"/>
@@ -1451,7 +1458,7 @@
       <c r="F26" s="6">
         <v>49</v>
       </c>
-      <c r="G26" s="26"/>
+      <c r="G26" s="25"/>
       <c r="H26" s="6" t="s">
         <v>66</v>
       </c>
@@ -1459,7 +1466,7 @@
       <c r="J26" s="6">
         <v>74</v>
       </c>
-      <c r="K26" s="19"/>
+      <c r="K26" s="18"/>
       <c r="L26" s="6" t="s">
         <v>25</v>
       </c>
@@ -1478,7 +1485,7 @@
       <c r="F27" s="6">
         <v>50</v>
       </c>
-      <c r="G27" s="26"/>
+      <c r="G27" s="25"/>
       <c r="H27" s="6" t="s">
         <v>68</v>
       </c>
@@ -1486,7 +1493,7 @@
       <c r="J27" s="6">
         <v>75</v>
       </c>
-      <c r="K27" s="19"/>
+      <c r="K27" s="18"/>
       <c r="L27" s="6" t="s">
         <v>24</v>
       </c>
@@ -1505,7 +1512,7 @@
       <c r="F28" s="6">
         <v>51</v>
       </c>
-      <c r="G28" s="26"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="6" t="s">
         <v>70</v>
       </c>
@@ -1513,7 +1520,7 @@
       <c r="J28" s="6">
         <v>76</v>
       </c>
-      <c r="K28" s="19"/>
+      <c r="K28" s="18"/>
       <c r="L28" s="6" t="s">
         <v>27</v>
       </c>
@@ -1529,18 +1536,18 @@
         <v>67</v>
       </c>
       <c r="E29" s="6"/>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24" t="s">
+      <c r="G29" s="23"/>
+      <c r="H29" s="23" t="s">
         <v>73</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6">
         <v>77</v>
       </c>
-      <c r="K29" s="19"/>
+      <c r="K29" s="18"/>
       <c r="L29" s="6" t="s">
         <v>69</v>
       </c>
@@ -1559,7 +1566,7 @@
       <c r="F30" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="27"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="11" t="s">
         <v>74</v>
       </c>
@@ -1586,7 +1593,7 @@
       <c r="F31" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G31" s="27"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="8" t="s">
         <v>75</v>
       </c>
@@ -1613,7 +1620,7 @@
       <c r="J32" s="11">
         <v>80</v>
       </c>
-      <c r="K32" s="20"/>
+      <c r="K32" s="19"/>
       <c r="L32" s="11" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
Sudden Day [Commit 1]
</commit_message>
<xml_diff>
--- a/Requisitos Bolsa de Trabajo.xlsx
+++ b/Requisitos Bolsa de Trabajo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alumno\Desktop\ProyectoA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\05. Integradora II\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -332,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +399,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -412,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -446,7 +452,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -467,13 +472,17 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,7 +795,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,44 +832,44 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="30" t="s">
         <v>82</v>
       </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5" t="s">
+      <c r="F3" s="30" t="s">
         <v>83</v>
       </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5" t="s">
+      <c r="J3" s="30" t="s">
         <v>84</v>
       </c>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -888,11 +897,11 @@
         <v>3</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="19">
+      <c r="F5" s="18">
         <v>27</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19" t="s">
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="5"/>
@@ -918,7 +927,7 @@
       <c r="F6" s="5">
         <v>28</v>
       </c>
-      <c r="G6" s="30"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
@@ -946,7 +955,7 @@
       <c r="F7" s="5">
         <v>29</v>
       </c>
-      <c r="G7" s="21"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="5" t="s">
         <v>9</v>
       </c>
@@ -971,11 +980,11 @@
         <v>11</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="19">
+      <c r="F8" s="18">
         <v>30</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19" t="s">
+      <c r="G8" s="18"/>
+      <c r="H8" s="18" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="5"/>
@@ -1001,7 +1010,7 @@
       <c r="F9" s="5">
         <v>31</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1037,7 @@
       <c r="F10" s="5">
         <v>32</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1047,7 +1056,7 @@
       <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="24"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
@@ -1055,7 +1064,7 @@
       <c r="F11" s="5">
         <v>33</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1082,7 +1091,7 @@
       <c r="F12" s="5">
         <v>34</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1109,7 +1118,7 @@
       <c r="F13" s="5">
         <v>35</v>
       </c>
-      <c r="G13" s="18"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="5" t="s">
         <v>26</v>
       </c>
@@ -1133,11 +1142,11 @@
         <v>24</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="19">
+      <c r="F14" s="18">
         <v>36</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19" t="s">
+      <c r="G14" s="18"/>
+      <c r="H14" s="18" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="5"/>
@@ -1163,7 +1172,7 @@
       <c r="F15" s="5">
         <v>37</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="5" t="s">
         <v>30</v>
       </c>
@@ -1190,7 +1199,7 @@
       <c r="F16" s="5">
         <v>38</v>
       </c>
-      <c r="G16" s="20"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="5" t="s">
         <v>33</v>
       </c>
@@ -1217,16 +1226,16 @@
       <c r="F17" s="5">
         <v>39</v>
       </c>
-      <c r="G17" s="21"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="I17" s="5"/>
-      <c r="J17" s="17">
+      <c r="J17" s="1">
         <v>64</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17" t="s">
+      <c r="K17" s="31"/>
+      <c r="L17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M17" s="5"/>
@@ -1244,7 +1253,7 @@
       <c r="F18" s="5">
         <v>40</v>
       </c>
-      <c r="G18" s="21"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="5" t="s">
         <v>39</v>
       </c>
@@ -1268,11 +1277,11 @@
         <v>41</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="19">
+      <c r="F19" s="18">
         <v>41</v>
       </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19" t="s">
+      <c r="G19" s="18"/>
+      <c r="H19" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I19" s="5"/>
@@ -1298,7 +1307,7 @@
       <c r="F20" s="5">
         <v>42</v>
       </c>
-      <c r="G20" s="21"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="5" t="s">
         <v>45</v>
       </c>
@@ -1325,7 +1334,7 @@
       <c r="F21" s="5">
         <v>43</v>
       </c>
-      <c r="G21" s="21"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="5" t="s">
         <v>48</v>
       </c>
@@ -1352,7 +1361,7 @@
       <c r="F22" s="5">
         <v>44</v>
       </c>
-      <c r="G22" s="21"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="5" t="s">
         <v>51</v>
       </c>
@@ -1379,7 +1388,7 @@
       <c r="F23" s="5">
         <v>45</v>
       </c>
-      <c r="G23" s="21"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="5" t="s">
         <v>57</v>
       </c>
@@ -1395,18 +1404,18 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="17">
+      <c r="B24" s="1">
         <v>20</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5">
         <v>46</v>
       </c>
-      <c r="G24" s="21"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="5" t="s">
         <v>60</v>
       </c>
@@ -1433,7 +1442,7 @@
       <c r="F25" s="5">
         <v>47</v>
       </c>
-      <c r="G25" s="21"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="5" t="s">
         <v>63</v>
       </c>
@@ -1457,11 +1466,11 @@
         <v>59</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="19">
+      <c r="F26" s="18">
         <v>48</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19" t="s">
+      <c r="G26" s="18"/>
+      <c r="H26" s="18" t="s">
         <v>64</v>
       </c>
       <c r="I26" s="5"/>
@@ -1487,7 +1496,7 @@
       <c r="F27" s="5">
         <v>49</v>
       </c>
-      <c r="G27" s="21"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="5" t="s">
         <v>66</v>
       </c>
@@ -1514,7 +1523,7 @@
       <c r="F28" s="5">
         <v>50</v>
       </c>
-      <c r="G28" s="21"/>
+      <c r="G28" s="20"/>
       <c r="H28" s="5" t="s">
         <v>68</v>
       </c>
@@ -1541,7 +1550,7 @@
       <c r="F29" s="5">
         <v>51</v>
       </c>
-      <c r="G29" s="21"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="5" t="s">
         <v>70</v>
       </c>
@@ -1565,11 +1574,11 @@
         <v>67</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19" t="s">
+      <c r="G30" s="18"/>
+      <c r="H30" s="18" t="s">
         <v>73</v>
       </c>
       <c r="I30" s="5"/>
@@ -1595,7 +1604,7 @@
       <c r="F31" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G31" s="22"/>
+      <c r="G31" s="21"/>
       <c r="H31" s="10" t="s">
         <v>74</v>
       </c>
@@ -1611,18 +1620,18 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27" t="s">
+      <c r="C32" s="25"/>
+      <c r="D32" s="26" t="s">
         <v>81</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G32" s="29"/>
+      <c r="G32" s="27"/>
       <c r="H32" s="7" t="s">
         <v>75</v>
       </c>
@@ -1684,11 +1693,11 @@
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
-      <c r="J35" s="25" t="s">
+      <c r="J35" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="K35" s="26"/>
-      <c r="L35" s="27" t="s">
+      <c r="K35" s="25"/>
+      <c r="L35" s="26" t="s">
         <v>81</v>
       </c>
       <c r="M35" s="5"/>
@@ -1724,10 +1733,13 @@
       <c r="M37" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>